<commit_message>
Organização de tarefas - task4
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32400A15-8A34-4599-8A68-103CE52797B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275F1C7-DA9D-48A0-A20B-5516351B8917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -338,6 +338,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,23 +365,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3013,7 +3013,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3029,24 +3029,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3059,18 +3059,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3093,161 +3093,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="17" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="18"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3270,176 +3284,143 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="19"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="22"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="22"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="17"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="18"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="18"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="19"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="19"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3456,6 +3437,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3485,24 +3499,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3515,18 +3529,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3549,147 +3563,147 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="17"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="17"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="18"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="7"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3712,151 +3726,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="19"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="22"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="22"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="17"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="18"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="18"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="19"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="19"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="21"/>
+      <c r="D43" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="19"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3873,107 +3887,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="11"/>
-      <c r="B45" s="14"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="14"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="17"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="15"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="15"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="18"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="15"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="18"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="16"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="19"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="19"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="20"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="21"/>
+      <c r="D54" s="12"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="21"/>
+      <c r="D55" s="12"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="22"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="14"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="15"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="18"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="15"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="18"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="16"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="19"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -3990,55 +4053,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task5
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275F1C7-DA9D-48A0-A20B-5516351B8917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237110A4-6CD3-44F5-9F51-C80B5F3B7881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -338,15 +338,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,14 +356,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3012,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF609A8-78B1-4901-B1B0-E5F68A46A5C6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3029,24 +3029,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3059,18 +3059,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3093,175 +3093,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="17" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="18"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="19"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="17" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="17" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="19"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="16"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="17" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17" t="s">
+      <c r="G19" s="11"/>
+      <c r="H19" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="18"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="18"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="15"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3284,143 +3284,190 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="17"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="17"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="15"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="18"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="18"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="18"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="17"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="17"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="14"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="18"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="18"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="18"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
-      <c r="B34" s="7"/>
-      <c r="D34" s="11"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="20"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="7"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="21"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="7"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="21"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
-      <c r="B37" s="8"/>
-      <c r="D37" s="13"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="22"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="17"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="17"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="18"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="18"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="18"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="18"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="15"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="16"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3437,39 +3484,6 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3499,24 +3513,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3529,18 +3543,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3563,147 +3577,147 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="17"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="18"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="19"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="17"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="19"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="16"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="7"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="17"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="18"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="18"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="15"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3726,151 +3740,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="17"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="17"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="15"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="18"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="18"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="18"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="17"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="17"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="14"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="14"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="18"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="18"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="18"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="12"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="13"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="17"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="17"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="14"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="18"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="18"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="18"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="18"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="15"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="16"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="B43" s="19"/>
+      <c r="D43" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3887,156 +3901,107 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="17"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="15"/>
-      <c r="B46" s="18"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="18"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="15"/>
-      <c r="B47" s="18"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="18"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="15"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="16"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="17"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="14"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="18"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="15"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="18"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="15"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="16"/>
-      <c r="B52" s="19"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="19"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="11"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="11"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="12"/>
+      <c r="D54" s="21"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="21"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="13"/>
+      <c r="D56" s="22"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="17"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="18"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="15"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="18"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="15"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="16"/>
-      <c r="B60" s="19"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="19"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4053,6 +4018,55 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas task6
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237110A4-6CD3-44F5-9F51-C80B5F3B7881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667618E8-AF8F-447F-9760-56B31776EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -338,6 +338,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,23 +365,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3013,7 +3013,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E38" sqref="E38:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3029,24 +3029,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3059,18 +3059,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3093,175 +3093,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="18"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="14"/>
+      <c r="H19" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3284,190 +3284,171 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="19"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="7"/>
-      <c r="G34" s="20"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="11"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="12"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="12"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="8"/>
-      <c r="G37" s="22"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="13"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="18"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="18"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="19"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="19"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3484,6 +3465,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3513,24 +3527,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3543,18 +3557,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="21"/>
+      <c r="D5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="21"/>
+      <c r="G5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3577,147 +3591,147 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="17"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="17"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="18"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="7"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3740,151 +3754,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="18"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="19"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="22"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="22"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="17"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="18"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="18"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="19"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="19"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="21"/>
+      <c r="D43" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="19"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3901,107 +3915,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="11"/>
-      <c r="B45" s="14"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="14"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="17"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="15"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="15"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="18"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="15"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="18"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="16"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="19"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="19"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="20"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="21"/>
+      <c r="D54" s="12"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="21"/>
+      <c r="D55" s="12"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="22"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="14"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="15"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="18"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="15"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="18"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="16"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="19"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4018,55 +4081,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task7
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667618E8-AF8F-447F-9760-56B31776EF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E7F74-595D-4A70-8A24-4068F148B51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -338,15 +338,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,14 +356,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3013,7 +3013,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E41"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3029,24 +3029,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3059,18 +3059,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3093,175 +3093,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="17" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="18"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="19"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="17" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="17" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="19"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="16"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="17" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17" t="s">
+      <c r="G19" s="11"/>
+      <c r="H19" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="18"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="18"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="15"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3284,171 +3284,218 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="17" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="17"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="15"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="18"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="18"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="18"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="11"/>
+      <c r="E30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="17"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="18"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="18"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="18"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="7"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="7"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="7"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="13"/>
-      <c r="H37" s="8"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="17" t="s">
+      <c r="D38" s="11"/>
+      <c r="E38" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="17"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="18"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="18"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="18"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="18"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="15"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="16"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3465,39 +3512,6 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3527,24 +3541,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3557,18 +3571,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3591,147 +3605,147 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="17"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="18"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="18"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="19"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="17"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="19"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="19"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="16"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="7"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="17"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="18"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="18"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="18"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="15"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="16"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3754,151 +3768,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="17"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="17"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="15"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="18"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="18"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="18"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="16"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="17"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="17"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="14"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="14"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="18"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="18"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="18"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="12"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="13"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="17"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="17"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="14"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="18"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="18"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="18"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="18"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="18"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="18"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="15"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="16"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="B43" s="19"/>
+      <c r="D43" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3915,156 +3929,107 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="17"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="15"/>
-      <c r="B46" s="18"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="18"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="15"/>
-      <c r="B47" s="18"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="18"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="15"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="16"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="17"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="14"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="18"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="15"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="18"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="15"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="16"/>
-      <c r="B52" s="19"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="19"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="11"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="11"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="12"/>
+      <c r="D54" s="21"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="21"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="13"/>
+      <c r="D56" s="22"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="17"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="18"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="15"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="18"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="15"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="16"/>
-      <c r="B60" s="19"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="19"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4081,6 +4046,55 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task8
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E7F74-595D-4A70-8A24-4068F148B51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59323C4D-CDE4-4921-99F3-7B3B9CC179AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
   <sheets>
     <sheet name="Bloco 02" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -169,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -286,31 +286,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,11 +312,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,23 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3012,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF609A8-78B1-4901-B1B0-E5F68A46A5C6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3028,29 +3002,33 @@
     <col min="8" max="8" width="46.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="H1" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -3093,160 +3071,160 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="12"/>
+      <c r="H19" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -3284,218 +3262,185 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14" t="s">
+      <c r="G26" s="12"/>
+      <c r="H26" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14" t="s">
+      <c r="G30" s="12"/>
+      <c r="H30" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="20"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="20"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="21"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="22"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="22"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14" t="s">
+      <c r="G38" s="12"/>
+      <c r="H38" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3512,6 +3457,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3524,7 +3502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
@@ -3540,29 +3518,33 @@
     <col min="8" max="8" width="46.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="H1" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -3605,132 +3587,146 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="16"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
-      <c r="B15" s="7"/>
-      <c r="D15" s="20"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="7"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="7"/>
-      <c r="D16" s="21"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="10"/>
       <c r="E16" s="7"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="7"/>
-      <c r="D17" s="21"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="7"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
-      <c r="B18" s="8"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="11"/>
       <c r="E18" s="8"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="16"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -3768,140 +3764,140 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="15"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="15"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="15"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="21"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="22"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="22"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="14"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="14"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="15"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="15"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="15"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="15"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="15"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -3929,107 +3925,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="11"/>
-      <c r="B45" s="14"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="14"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="15"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="15"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="16"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="17"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="14"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="15"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="15"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="15"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="16"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="15"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="16"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="20"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="9"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="21"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="21"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="22"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="14"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="15"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="15"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="15"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="16"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="17"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4046,55 +4091,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task9
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59323C4D-CDE4-4921-99F3-7B3B9CC179AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA7BDF0-7D19-41EF-84C0-31AFA6CC7539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -312,15 +312,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,14 +330,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3003,13 +3003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3018,11 +3018,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3037,18 +3037,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="17"/>
+      <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3071,175 +3071,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="16"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="16"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="17"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="15" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="17"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="17"/>
+      <c r="D24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="17"/>
+      <c r="G24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3262,185 +3262,218 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="15" t="s">
+      <c r="G26" s="9"/>
+      <c r="H26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="17"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="15" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="15" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="17"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="14"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="9"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="10"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="10"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="11"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="11"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="15" t="s">
+      <c r="G38" s="9"/>
+      <c r="H38" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="16"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="13"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="17"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3457,39 +3490,6 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3502,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3519,13 +3519,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3534,11 +3534,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3553,18 +3553,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="17"/>
+      <c r="G5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3587,161 +3587,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="15"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="16"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="15"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="16"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="17"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="18"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="7"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="19"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="7"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="19"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="8"/>
-      <c r="G18" s="11"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="15"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="17"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="17"/>
+      <c r="D24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="17"/>
+      <c r="G24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3764,151 +3778,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="15"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="17"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="15"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="15"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="12"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="17"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="14"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="9"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="9"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="10"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="15"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="15"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="15"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="12"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="12"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="16"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="13"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="17"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="17"/>
+      <c r="D43" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="19"/>
+      <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3925,156 +3939,107 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="15"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="16"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="16"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="14"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="17"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="15"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="15"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="12"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
-      <c r="B50" s="16"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="16"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="16"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="17"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="9"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="9"/>
+      <c r="D53" s="18"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="10"/>
+      <c r="D54" s="19"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="10"/>
+      <c r="D55" s="19"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="11"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="11"/>
+      <c r="D56" s="20"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="15"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="12"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="16"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="13"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="16"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14"/>
-      <c r="B60" s="17"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="17"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="14"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4091,6 +4056,55 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task10
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA7BDF0-7D19-41EF-84C0-31AFA6CC7539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D3D745-8A9E-4270-B5F2-35F890848848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -312,6 +312,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,23 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2986,7 +2986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF609A8-78B1-4901-B1B0-E5F68A46A5C6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H38" sqref="H38:H41"/>
     </sheetView>
   </sheetViews>
@@ -3003,13 +3003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3018,11 +3018,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3037,18 +3037,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3071,175 +3071,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="12" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="18"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12" t="s">
+      <c r="G19" s="12"/>
+      <c r="H19" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3262,218 +3262,185 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12" t="s">
+      <c r="G26" s="12"/>
+      <c r="H26" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="12" t="s">
+      <c r="G30" s="12"/>
+      <c r="H30" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="20"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="20"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="12" t="s">
+      <c r="G38" s="12"/>
+      <c r="H38" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="13"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="13"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="13"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="14"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3490,6 +3457,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3502,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3519,13 +3519,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3534,11 +3534,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3553,18 +3553,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3587,175 +3587,189 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="12" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3778,151 +3792,151 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="12"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="12"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="15"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7"/>
-      <c r="D34" s="18"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="18"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7"/>
-      <c r="D35" s="19"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="19"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7"/>
-      <c r="D36" s="19"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="19"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="20"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="12"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="12"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="15"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="15"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="13"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="13"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="13"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="14"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="D43" s="16" t="s">
+      <c r="B43" s="19"/>
+      <c r="D43" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="17"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3939,107 +3953,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="10"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="11"/>
-      <c r="B48" s="14"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="17"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="12"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="12"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="15"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="13"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="13"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="16"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="13"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="13"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="11"/>
-      <c r="B52" s="14"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="14"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="18"/>
+      <c r="D53" s="9"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="19"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="19"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="19"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="19"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="20"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="20"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="12"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="12"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="15"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="13"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="13"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
-      <c r="B59" s="13"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="13"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="11"/>
-      <c r="B60" s="14"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="14"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="17"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4056,55 +4119,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task11
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D3D745-8A9E-4270-B5F2-35F890848848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA361349-A6C2-4B5C-937D-B9A4987F542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -312,15 +312,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,14 +330,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3003,13 +3003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3018,11 +3018,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3037,18 +3037,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="17"/>
+      <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3071,175 +3071,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="16"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="16"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="17"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="15" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="17"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="17"/>
+      <c r="D24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="17"/>
+      <c r="G24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3262,185 +3262,218 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="15" t="s">
+      <c r="G26" s="9"/>
+      <c r="H26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="17"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="15" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="15" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="17"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="14"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="9"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="10"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="10"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="11"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="11"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="15" t="s">
+      <c r="G38" s="9"/>
+      <c r="H38" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="16"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="13"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="17"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3457,39 +3490,6 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3502,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3519,13 +3519,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3534,11 +3534,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3553,18 +3553,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="17"/>
+      <c r="G5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3587,189 +3587,189 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="16"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="16"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="17"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="17"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="14"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="D24" s="18" t="s">
+      <c r="B24" s="17"/>
+      <c r="D24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="17"/>
+      <c r="G24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3792,151 +3792,165 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="15"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="17"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="15"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="15"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="12"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="17"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="14"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
-      <c r="B34" s="7"/>
-      <c r="D34" s="9"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="18"/>
       <c r="E34" s="7"/>
-      <c r="G34" s="9"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
-      <c r="B35" s="7"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="19"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
-      <c r="B36" s="7"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="19"/>
       <c r="E36" s="7"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
-      <c r="B37" s="8"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="20"/>
       <c r="E37" s="8"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="15"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="15"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="15"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="12"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="16"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="16"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="13"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="17"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="17"/>
+      <c r="D43" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="19"/>
+      <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3953,156 +3967,107 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="15"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="16"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="16"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="14"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="17"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="15"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="15"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="12"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
-      <c r="B50" s="16"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="16"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="16"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="17"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="9"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="9"/>
+      <c r="D53" s="18"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="10"/>
+      <c r="D54" s="19"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="10"/>
+      <c r="D55" s="19"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="11"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="11"/>
+      <c r="D56" s="20"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="15"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="12"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="16"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="13"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="16"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14"/>
-      <c r="B60" s="17"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="17"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="14"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4119,6 +4084,55 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Organização de tarefas - task12
</commit_message>
<xml_diff>
--- a/Organização de tarefas (ColaboraTech).xlsx
+++ b/Organização de tarefas (ColaboraTech).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mariana\Estudos\2022 Bootcamp Java (Generation Brasil)\ProjetoIntegrador\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA361349-A6C2-4B5C-937D-B9A4987F542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7117F573-1450-4FE9-ADDD-57B373C1C6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8A1726B6-E61D-48E4-974C-11473AA94446}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="26">
   <si>
     <t>TASK 03</t>
   </si>
@@ -312,6 +312,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,23 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3003,13 +3003,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3018,11 +3018,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3037,18 +3037,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3071,175 +3071,175 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="12" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7"/>
-      <c r="D15" s="18"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="8"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12" t="s">
+      <c r="G19" s="12"/>
+      <c r="H19" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3262,218 +3262,185 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12" t="s">
+      <c r="G26" s="12"/>
+      <c r="H26" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="12" t="s">
+      <c r="G30" s="12"/>
+      <c r="H30" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="20"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="20"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="12" t="s">
+      <c r="G38" s="12"/>
+      <c r="H38" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="13"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="13"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="13"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="14"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="B1:F2"/>
@@ -3490,6 +3457,39 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3502,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B67CF-FE7D-44E4-A9DC-635976C3C237}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3519,13 +3519,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3534,11 +3534,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3553,18 +3553,18 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="19"/>
+      <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="G5" s="16" t="s">
+      <c r="E5" s="19"/>
+      <c r="G5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3587,189 +3587,189 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="12" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12" t="s">
+      <c r="G19" s="12"/>
+      <c r="H19" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="16"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="16"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="14"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="14"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="17"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="G24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
@@ -3792,165 +3792,179 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="12"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="7"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="9"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="7"/>
-      <c r="G35" s="19"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="10"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="7"/>
-      <c r="G36" s="19"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="10"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="8"/>
-      <c r="G37" s="20"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="11"/>
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="12"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="13"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="13"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="13"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="14"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="D43" s="16" t="s">
+      <c r="B43" s="19"/>
+      <c r="D43" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="17"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
@@ -3967,107 +3981,156 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="10"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="11"/>
-      <c r="B48" s="14"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="17"/>
     </row>
     <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="12"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="12"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="15"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="13"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="13"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="16"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="13"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="13"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="11"/>
-      <c r="B52" s="14"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="14"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="7"/>
-      <c r="D53" s="18"/>
+      <c r="D53" s="9"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="19"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="7"/>
-      <c r="D54" s="19"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="19"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="7"/>
-      <c r="D55" s="19"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="20"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="8"/>
-      <c r="D56" s="20"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="12"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="12"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="15"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="13"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="13"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
-      <c r="B59" s="13"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="13"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="11"/>
-      <c r="B60" s="14"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="14"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="17"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
@@ -4084,55 +4147,6 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>